<commit_message>
Test de generacion de archivo de movimientos
</commit_message>
<xml_diff>
--- a/economizate/dominio/src/test/resources/movimientos.xlsx
+++ b/economizate/dominio/src/test/resources/movimientos.xlsx
@@ -12,7 +12,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+  <si>
+    <t>27/04/2018</t>
+  </si>
   <si>
     <t>Luz</t>
   </si>
@@ -68,7 +71,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -81,18 +84,24 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="n">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="n">
         <v>-300.0</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="n">
         <v>37214.52</v>
       </c>
     </row>

</xml_diff>

<commit_message>
tests us 4 listas
</commit_message>
<xml_diff>
--- a/economizate/dominio/src/test/resources/movimientos.xlsx
+++ b/economizate/dominio/src/test/resources/movimientos.xlsx
@@ -12,21 +12,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
-    <t>27/04/2018</t>
+    <t>15/03/2018</t>
+  </si>
+  <si>
+    <t>cuenta sueldo</t>
+  </si>
+  <si>
+    <t>ninguna</t>
+  </si>
+  <si>
+    <t>31/03/2018</t>
+  </si>
+  <si>
+    <t>horas extras</t>
+  </si>
+  <si>
+    <t>13/04/2018</t>
   </si>
   <si>
     <t>Luz</t>
   </si>
   <si>
-    <t>Abril</t>
+    <t>Servicio</t>
+  </si>
+  <si>
+    <t>26/04/2018</t>
+  </si>
+  <si>
+    <t>Gas</t>
+  </si>
+  <si>
+    <t>18/04/2018</t>
   </si>
   <si>
     <t>Sueldo</t>
   </si>
   <si>
-    <t>Me descontaron ganancias</t>
+    <t>23/04/2018</t>
+  </si>
+  <si>
+    <t>Tarjeta</t>
+  </si>
+  <si>
+    <t>Gastos Generales</t>
   </si>
 </sst>
 </file>
@@ -71,7 +101,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -88,21 +118,77 @@
         <v>2</v>
       </c>
       <c r="D1" t="n">
-        <v>-300.0</v>
+        <v>95.0</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D2" t="n">
-        <v>37214.52</v>
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-15.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-15.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="n">
+        <v>95.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-70.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>